<commit_message>
Working on expired debts report
</commit_message>
<xml_diff>
--- a/application/views/plugins/reports/Expired_debts/Expired_debts.xlsx
+++ b/application/views/plugins/reports/Expired_debts/Expired_debts.xlsx
@@ -14,54 +14,81 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>Всего</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Группа</t>
   </si>
   <si>
-    <t>Оплаты и отгрузки клиентам</t>
-  </si>
-  <si>
-    <t>Дата</t>
-  </si>
-  <si>
-    <t>Клиент</t>
-  </si>
-  <si>
-    <t>Пояснение</t>
-  </si>
-  <si>
-    <t>Отгрузка</t>
-  </si>
-  <si>
-    <t>Оплата</t>
-  </si>
-  <si>
-    <t>{$v-&gt;rows[]-&gt;cdate}</t>
-  </si>
-  <si>
     <t>{$v-&gt;rows[]-&gt;label}</t>
   </si>
   <si>
-    <t>{$v-&gt;rows[]-&gt;description}</t>
-  </si>
-  <si>
-    <t>{$v-&gt;rows[]-&gt;debit}</t>
-  </si>
-  <si>
-    <t>{$v-&gt;rows[]-&gt;credit}</t>
-  </si>
-  <si>
     <t>{$v-&gt;rows[]-&gt;path}</t>
   </si>
   <si>
-    <t>{$v-&gt;total_debit}</t>
-  </si>
-  <si>
-    <t>{$v-&gt;total_credit}</t>
+    <t>Задолженность клиентов</t>
+  </si>
+  <si>
+    <t>Наш долг</t>
+  </si>
+  <si>
+    <t>Компания</t>
+  </si>
+  <si>
+    <t>Их долг</t>
+  </si>
+  <si>
+    <t>Общий</t>
+  </si>
+  <si>
+    <t>Просроченный</t>
+  </si>
+  <si>
+    <t>Отсрочка</t>
+  </si>
+  <si>
+    <t>Просрочка</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;buy}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;sell}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;exp}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;deferment}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;m}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;d}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;total_our_debt}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;total_their_debt}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;total_their_exp}</t>
+  </si>
+  <si>
+    <t>мес.</t>
+  </si>
+  <si>
+    <t>дн.</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;phone}</t>
+  </si>
+  <si>
+    <t>Название</t>
+  </si>
+  <si>
+    <t>Телефон</t>
   </si>
 </sst>
 </file>
@@ -104,7 +131,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF00B050"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -112,7 +139,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -121,7 +147,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -129,7 +154,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="4" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -156,7 +181,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -273,19 +298,6 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -303,6 +315,58 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -313,7 +377,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -321,8 +385,8 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -333,40 +397,58 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -673,98 +755,149 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G6"/>
+  <dimension ref="B1:J7"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E5"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.28515625" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" customWidth="1"/>
-    <col min="4" max="4" width="35" customWidth="1"/>
-    <col min="5" max="7" width="14.85546875" customWidth="1"/>
+    <col min="2" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="6" width="15" customWidth="1"/>
+    <col min="7" max="8" width="5.42578125" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" customWidth="1"/>
+    <col min="10" max="10" width="30.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:10" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
-      <c r="G2" s="8"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="8"/>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="4" t="s">
+    <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="9"/>
+      <c r="G3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="9"/>
+      <c r="I3" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="E4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="20"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="13"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="5"/>
+    </row>
+    <row r="6" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="26" t="s">
         <v>1</v>
       </c>
+      <c r="C6" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="27" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="10"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="1"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="3"/>
+    <row r="7" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="1"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B4:D4"/>
+  <mergeCells count="4">
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="B3:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>